<commit_message>
Added data driven testing to Login class
</commit_message>
<xml_diff>
--- a/bin/data/testfile.xlsx
+++ b/bin/data/testfile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>User</t>
   </si>
@@ -19,10 +19,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>test</t>
+    <t>mcAngular</t>
   </si>
   <si>
-    <t>1234</t>
+    <t>3d6g4f7j5g8k</t>
+  </si>
+  <si>
+    <t>tmtmoney</t>
+  </si>
+  <si>
+    <t>oy06ri94uw73</t>
   </si>
 </sst>
 </file>
@@ -51,14 +57,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -95,8 +98,16 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>